<commit_message>
inserita tabella nel file word
</commit_message>
<xml_diff>
--- a/RESULTS.xlsx
+++ b/RESULTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afasu\Google Drive\MASTER DATA SCIENCE\ESAMI\2. Economic and Financial Data Science\mds_causal_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81FB036-C634-4195-8D23-9ECC6B42D0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD1BB77-3A1F-48F7-A1F2-F17A563A22B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,6 +389,15 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,15 +408,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -721,7 +721,7 @@
   <dimension ref="B3:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,39 +734,39 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -971,7 +971,7 @@
       <c r="G12" s="5">
         <v>0.24229999999999999</v>
       </c>
-      <c r="H12" s="11" t="b">
+      <c r="H12" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="4" t="b">
@@ -1075,7 +1075,7 @@
       <c r="G16" s="5">
         <v>0</v>
       </c>
-      <c r="H16" s="11" t="b">
+      <c r="H16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I16" s="4" t="b">
@@ -1101,7 +1101,7 @@
       <c r="G17" s="5">
         <v>0</v>
       </c>
-      <c r="H17" s="11" t="b">
+      <c r="H17" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I17" s="4" t="b">
@@ -1153,7 +1153,7 @@
       <c r="G19" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H19" s="11" t="b">
+      <c r="H19" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I19" s="4" t="b">
@@ -1257,7 +1257,7 @@
       <c r="G23" s="5">
         <v>8.7099999999999997E-2</v>
       </c>
-      <c r="H23" s="11" t="b">
+      <c r="H23" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I23" s="4" t="b">
@@ -1413,10 +1413,10 @@
       <c r="G29" s="5">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="H29" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="12" t="b">
+      <c r="H29" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1439,10 +1439,10 @@
       <c r="G30" s="5">
         <v>1.43E-2</v>
       </c>
-      <c r="H30" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="12" t="b">
+      <c r="H30" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1465,7 +1465,7 @@
       <c r="G31" s="5">
         <v>0.54979999999999996</v>
       </c>
-      <c r="H31" s="11" t="b">
+      <c r="H31" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I31" s="4" t="b">
@@ -1517,7 +1517,7 @@
       <c r="G33" s="5">
         <v>0.77400000000000002</v>
       </c>
-      <c r="H33" s="11" t="b">
+      <c r="H33" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I33" s="4" t="b">
@@ -1595,7 +1595,7 @@
       <c r="G36" s="5">
         <v>5.9799999999999999E-2</v>
       </c>
-      <c r="H36" s="11" t="b">
+      <c r="H36" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I36" s="4" t="b">
@@ -1647,7 +1647,7 @@
       <c r="G38" s="5">
         <v>0.2273</v>
       </c>
-      <c r="H38" s="11" t="b">
+      <c r="H38" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I38" s="4" t="b">
@@ -1699,7 +1699,7 @@
       <c r="G40" s="5">
         <v>9.1700000000000004E-2</v>
       </c>
-      <c r="H40" s="11" t="b">
+      <c r="H40" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I40" s="4" t="b">
@@ -1907,10 +1907,10 @@
       <c r="G48" s="5">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="H48" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="12" t="b">
+      <c r="H48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2141,10 +2141,10 @@
       <c r="G57" s="5">
         <v>1.95E-2</v>
       </c>
-      <c r="H57" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="12" t="b">
+      <c r="H57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2245,10 +2245,10 @@
       <c r="G61" s="5">
         <v>3.09E-2</v>
       </c>
-      <c r="H61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I61" s="12" t="b">
+      <c r="H61" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2453,7 +2453,7 @@
       <c r="G69" s="5">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H69" s="11" t="b">
+      <c r="H69" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I69" s="4" t="b">
@@ -2479,10 +2479,10 @@
       <c r="G70" s="5">
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="H70" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" s="12" t="b">
+      <c r="H70" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="8" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>